<commit_message>
Implemented Kilian for real and played around with P_K and LR restriction horizon
1. Implemented the Kilian correction for stationarity also
(bootstrap_with_kilian.m)
2. Played to get good results: excluded hours, put in price of capital
as a proxy for relative prices and as a last thing moved around the
horizon at which we impose the LR restriction. -> Conclusion: keep
hours out, they seem to screw things up; include P_K as a robustness
check b/c they are longer and a bit more cyclical than P_IT; decrease
LR restriction horizon —> gives reasonable FEV and can argue about IRFs.
</commit_message>
<xml_diff>
--- a/Data/dataset_23_sept_2017.xlsx
+++ b/Data/dataset_23_sept_2017.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="295">
   <si>
     <t>date</t>
   </si>
@@ -904,6 +904,9 @@
   </si>
   <si>
     <t>Consumer Price Index for All Urban Consumers: All Items, Index 1982-1984=100, Quarterly, Seasonally Adjusted</t>
+  </si>
+  <si>
+    <t>Price capital</t>
   </si>
 </sst>
 </file>
@@ -954,7 +957,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -967,6 +970,7 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1282,10 +1286,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K1999"/>
+  <dimension ref="A1:L1999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A265" workbookViewId="0">
-      <selection activeCell="K283" sqref="K283"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1295,9 +1299,10 @@
     <col min="6" max="6" width="8.83203125" style="3"/>
     <col min="8" max="8" width="8.83203125" style="3"/>
     <col min="10" max="10" width="8.83203125" style="3"/>
+    <col min="12" max="12" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1331,8 +1336,11 @@
       <c r="K1" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="L1" s="3" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1356,7 +1364,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1381,8 +1389,11 @@
       <c r="K3" s="7">
         <v>22.08</v>
       </c>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="L3" s="10">
+        <v>19.899999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1407,8 +1418,11 @@
       <c r="K4" s="7">
         <v>22.84</v>
       </c>
-    </row>
-    <row r="5" spans="1:11">
+      <c r="L4" s="10">
+        <v>20.100000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1433,8 +1447,11 @@
       <c r="K5" s="7">
         <v>23.41</v>
       </c>
-    </row>
-    <row r="6" spans="1:11">
+      <c r="L5" s="10">
+        <v>20.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1459,8 +1476,11 @@
       <c r="K6" s="7">
         <v>23.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:11">
+      <c r="L6" s="10">
+        <v>20.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1485,8 +1505,11 @@
       <c r="K7" s="7">
         <v>24.15</v>
       </c>
-    </row>
-    <row r="8" spans="1:11">
+      <c r="L7" s="10">
+        <v>21.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1511,8 +1534,11 @@
       <c r="K8" s="7">
         <v>24.36</v>
       </c>
-    </row>
-    <row r="9" spans="1:11">
+      <c r="L8" s="10">
+        <v>22.4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1537,8 +1563,11 @@
       <c r="K9" s="7">
         <v>24.05</v>
       </c>
-    </row>
-    <row r="10" spans="1:11">
+      <c r="L9" s="10">
+        <v>22.6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1563,8 +1592,11 @@
       <c r="K10" s="7">
         <v>23.91</v>
       </c>
-    </row>
-    <row r="11" spans="1:11">
+      <c r="L10" s="10">
+        <v>22.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1589,8 +1621,11 @@
       <c r="K11" s="7">
         <v>23.92</v>
       </c>
-    </row>
-    <row r="12" spans="1:11">
+      <c r="L11" s="10">
+        <v>22.9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1615,8 +1650,11 @@
       <c r="K12" s="7">
         <v>23.75</v>
       </c>
-    </row>
-    <row r="13" spans="1:11">
+      <c r="L12" s="10">
+        <v>22.6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1641,8 +1679,11 @@
       <c r="K13" s="7">
         <v>23.61</v>
       </c>
-    </row>
-    <row r="14" spans="1:11">
+      <c r="L13" s="10">
+        <v>22.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1667,8 +1708,11 @@
       <c r="K14" s="7">
         <v>23.64</v>
       </c>
-    </row>
-    <row r="15" spans="1:11">
+      <c r="L14" s="10">
+        <v>22.6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1693,8 +1737,11 @@
       <c r="K15" s="7">
         <v>23.88</v>
       </c>
-    </row>
-    <row r="16" spans="1:11">
+      <c r="L15" s="10">
+        <v>22.8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1719,8 +1766,11 @@
       <c r="K16" s="7">
         <v>24.34</v>
       </c>
-    </row>
-    <row r="17" spans="1:11">
+      <c r="L16" s="10">
+        <v>23.7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1745,8 +1795,11 @@
       <c r="K17" s="7">
         <v>24.98</v>
       </c>
-    </row>
-    <row r="18" spans="1:11">
+      <c r="L17" s="10">
+        <v>24.8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1771,8 +1824,11 @@
       <c r="K18" s="7">
         <v>25.88</v>
       </c>
-    </row>
-    <row r="19" spans="1:11">
+      <c r="L18" s="10">
+        <v>25.3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1797,8 +1853,11 @@
       <c r="K19" s="7">
         <v>25.93</v>
       </c>
-    </row>
-    <row r="20" spans="1:11">
+      <c r="L19" s="10">
+        <v>25.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1823,8 +1882,11 @@
       <c r="K20" s="7">
         <v>26.03</v>
       </c>
-    </row>
-    <row r="21" spans="1:11">
+      <c r="L20" s="10">
+        <v>25.6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1849,8 +1911,11 @@
       <c r="K21" s="7">
         <v>26.47</v>
       </c>
-    </row>
-    <row r="22" spans="1:11">
+      <c r="L21" s="10">
+        <v>25.7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1875,8 +1940,11 @@
       <c r="K22" s="7">
         <v>26.39</v>
       </c>
-    </row>
-    <row r="23" spans="1:11">
+      <c r="L22" s="10">
+        <v>25.9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1901,8 +1969,11 @@
       <c r="K23" s="7">
         <v>26.53</v>
       </c>
-    </row>
-    <row r="24" spans="1:11">
+      <c r="L23" s="10">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1927,8 +1998,11 @@
       <c r="K24" s="7">
         <v>26.63</v>
       </c>
-    </row>
-    <row r="25" spans="1:11">
+      <c r="L24" s="10">
+        <v>25.9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1953,8 +2027,11 @@
       <c r="K25" s="7">
         <v>26.71</v>
       </c>
-    </row>
-    <row r="26" spans="1:11">
+      <c r="L25" s="10">
+        <v>25.9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1979,8 +2056,11 @@
       <c r="K26" s="7">
         <v>26.63</v>
       </c>
-    </row>
-    <row r="27" spans="1:11">
+      <c r="L26" s="10">
+        <v>26.1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -2005,8 +2085,11 @@
       <c r="K27" s="7">
         <v>26.77</v>
       </c>
-    </row>
-    <row r="28" spans="1:11">
+      <c r="L27" s="10">
+        <v>26.4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -2031,8 +2114,11 @@
       <c r="K28" s="7">
         <v>26.89</v>
       </c>
-    </row>
-    <row r="29" spans="1:11">
+      <c r="L28" s="10">
+        <v>26.6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -2057,8 +2143,11 @@
       <c r="K29" s="7">
         <v>26.87</v>
       </c>
-    </row>
-    <row r="30" spans="1:11">
+      <c r="L29" s="10">
+        <v>26.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -2083,8 +2172,11 @@
       <c r="K30" s="7">
         <v>26.93</v>
       </c>
-    </row>
-    <row r="31" spans="1:11">
+      <c r="L30" s="10">
+        <v>26.6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -2109,8 +2201,11 @@
       <c r="K31" s="7">
         <v>26.94</v>
       </c>
-    </row>
-    <row r="32" spans="1:11">
+      <c r="L31" s="10">
+        <v>26.7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -2135,8 +2230,11 @@
       <c r="K32" s="7">
         <v>26.81</v>
       </c>
-    </row>
-    <row r="33" spans="1:11">
+      <c r="L32" s="10">
+        <v>26.6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -2161,8 +2259,11 @@
       <c r="K33" s="7">
         <v>26.77</v>
       </c>
-    </row>
-    <row r="34" spans="1:11">
+      <c r="L33" s="10">
+        <v>26.8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -2187,8 +2288,11 @@
       <c r="K34" s="7">
         <v>26.79</v>
       </c>
-    </row>
-    <row r="35" spans="1:11">
+      <c r="L34" s="10">
+        <v>26.9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -2213,8 +2317,11 @@
       <c r="K35" s="7">
         <v>26.71</v>
       </c>
-    </row>
-    <row r="36" spans="1:11">
+      <c r="L35" s="10">
+        <v>27.3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -2239,8 +2346,11 @@
       <c r="K36" s="7">
         <v>26.85</v>
       </c>
-    </row>
-    <row r="37" spans="1:11">
+      <c r="L36" s="10">
+        <v>27.8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -2265,8 +2375,11 @@
       <c r="K37" s="7">
         <v>26.87</v>
       </c>
-    </row>
-    <row r="38" spans="1:11">
+      <c r="L37" s="10">
+        <v>28.3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -2291,8 +2404,11 @@
       <c r="K38" s="7">
         <v>26.89</v>
       </c>
-    </row>
-    <row r="39" spans="1:11">
+      <c r="L38" s="10">
+        <v>28.8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -2317,8 +2433,11 @@
       <c r="K39" s="7">
         <v>27.15</v>
       </c>
-    </row>
-    <row r="40" spans="1:11">
+      <c r="L39" s="10">
+        <v>29.4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -2343,8 +2462,11 @@
       <c r="K40" s="7">
         <v>27.35</v>
       </c>
-    </row>
-    <row r="41" spans="1:11">
+      <c r="L40" s="10">
+        <v>30.1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -2369,8 +2491,11 @@
       <c r="K41" s="7">
         <v>27.63</v>
       </c>
-    </row>
-    <row r="42" spans="1:11">
+      <c r="L41" s="10">
+        <v>30.6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -2395,8 +2520,11 @@
       <c r="K42" s="7">
         <v>27.86</v>
       </c>
-    </row>
-    <row r="43" spans="1:11">
+      <c r="L42" s="10">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -2421,8 +2549,11 @@
       <c r="K43" s="7">
         <v>28.11</v>
       </c>
-    </row>
-    <row r="44" spans="1:11">
+      <c r="L43" s="10">
+        <v>31.2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -2447,8 +2578,11 @@
       <c r="K44" s="7">
         <v>28.32</v>
       </c>
-    </row>
-    <row r="45" spans="1:11">
+      <c r="L44" s="10">
+        <v>31.6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -2473,8 +2607,11 @@
       <c r="K45" s="7">
         <v>28.47</v>
       </c>
-    </row>
-    <row r="46" spans="1:11">
+      <c r="L45" s="10">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -2499,8 +2636,11 @@
       <c r="K46" s="7">
         <v>28.87</v>
       </c>
-    </row>
-    <row r="47" spans="1:11">
+      <c r="L46" s="10">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -2525,8 +2665,11 @@
       <c r="K47" s="7">
         <v>28.91</v>
       </c>
-    </row>
-    <row r="48" spans="1:11">
+      <c r="L47" s="10">
+        <v>32.1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -2551,8 +2694,11 @@
       <c r="K48" s="7">
         <v>28.91</v>
       </c>
-    </row>
-    <row r="49" spans="1:11">
+      <c r="L48" s="10">
+        <v>32.1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -2577,8 +2723,11 @@
       <c r="K49" s="7">
         <v>28.97</v>
       </c>
-    </row>
-    <row r="50" spans="1:11">
+      <c r="L49" s="10">
+        <v>32.4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -2603,8 +2752,11 @@
       <c r="K50" s="7">
         <v>28.97</v>
       </c>
-    </row>
-    <row r="51" spans="1:11">
+      <c r="L50" s="10">
+        <v>32.6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -2629,8 +2781,11 @@
       <c r="K51" s="7">
         <v>29.11</v>
       </c>
-    </row>
-    <row r="52" spans="1:11">
+      <c r="L51" s="10">
+        <v>32.9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -2655,8 +2810,11 @@
       <c r="K52" s="7">
         <v>29.25</v>
       </c>
-    </row>
-    <row r="53" spans="1:11">
+      <c r="L52" s="10">
+        <v>32.9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -2681,8 +2839,11 @@
       <c r="K53" s="7">
         <v>29.41</v>
       </c>
-    </row>
-    <row r="54" spans="1:11">
+      <c r="L53" s="10">
+        <v>32.700000000000003</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -2707,8 +2868,11 @@
       <c r="K54" s="7">
         <v>29.41</v>
       </c>
-    </row>
-    <row r="55" spans="1:11">
+      <c r="L54" s="10">
+        <v>32.9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -2733,8 +2897,11 @@
       <c r="K55" s="7">
         <v>29.61</v>
       </c>
-    </row>
-    <row r="56" spans="1:11">
+      <c r="L55" s="10">
+        <v>32.799999999999997</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -2759,8 +2926,11 @@
       <c r="K56" s="7">
         <v>29.61</v>
       </c>
-    </row>
-    <row r="57" spans="1:11">
+      <c r="L56" s="10">
+        <v>32.6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12">
       <c r="A57" t="s">
         <v>56</v>
       </c>
@@ -2785,8 +2955,11 @@
       <c r="K57" s="7">
         <v>29.81</v>
       </c>
-    </row>
-    <row r="58" spans="1:11">
+      <c r="L57" s="10">
+        <v>32.799999999999997</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12">
       <c r="A58" t="s">
         <v>57</v>
       </c>
@@ -2811,8 +2984,11 @@
       <c r="K58" s="7">
         <v>29.84</v>
       </c>
-    </row>
-    <row r="59" spans="1:11">
+      <c r="L58" s="10">
+        <v>32.9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12">
       <c r="A59" t="s">
         <v>58</v>
       </c>
@@ -2837,8 +3013,11 @@
       <c r="K59" s="7">
         <v>29.84</v>
       </c>
-    </row>
-    <row r="60" spans="1:11">
+      <c r="L59" s="10">
+        <v>32.9</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -2863,8 +3042,11 @@
       <c r="K60" s="7">
         <v>29.98</v>
       </c>
-    </row>
-    <row r="61" spans="1:11">
+      <c r="L60" s="10">
+        <v>32.9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -2889,8 +3071,11 @@
       <c r="K61" s="7">
         <v>30.01</v>
       </c>
-    </row>
-    <row r="62" spans="1:11">
+      <c r="L61" s="10">
+        <v>32.9</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12">
       <c r="A62" t="s">
         <v>61</v>
       </c>
@@ -2915,8 +3100,11 @@
       <c r="K62" s="7">
         <v>30.17</v>
       </c>
-    </row>
-    <row r="63" spans="1:11">
+      <c r="L62" s="10">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12">
       <c r="A63" t="s">
         <v>62</v>
       </c>
@@ -2941,8 +3129,11 @@
       <c r="K63" s="7">
         <v>30.21</v>
       </c>
-    </row>
-    <row r="64" spans="1:11">
+      <c r="L63" s="10">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12">
       <c r="A64" t="s">
         <v>63</v>
       </c>
@@ -2967,8 +3158,11 @@
       <c r="K64" s="7">
         <v>30.42</v>
       </c>
-    </row>
-    <row r="65" spans="1:11">
+      <c r="L64" s="10">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12">
       <c r="A65" t="s">
         <v>64</v>
       </c>
@@ -2993,8 +3187,11 @@
       <c r="K65" s="7">
         <v>30.38</v>
       </c>
-    </row>
-    <row r="66" spans="1:11">
+      <c r="L65" s="10">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12">
       <c r="A66" t="s">
         <v>65</v>
       </c>
@@ -3019,8 +3216,11 @@
       <c r="K66" s="7">
         <v>30.51</v>
       </c>
-    </row>
-    <row r="67" spans="1:11">
+      <c r="L66" s="10">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12">
       <c r="A67" t="s">
         <v>66</v>
       </c>
@@ -3045,8 +3245,11 @@
       <c r="K67" s="7">
         <v>30.61</v>
       </c>
-    </row>
-    <row r="68" spans="1:11">
+      <c r="L67" s="10">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12">
       <c r="A68" t="s">
         <v>67</v>
       </c>
@@ -3071,8 +3274,11 @@
       <c r="K68" s="7">
         <v>30.72</v>
       </c>
-    </row>
-    <row r="69" spans="1:11">
+      <c r="L68" s="10">
+        <v>33.1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12">
       <c r="A69" t="s">
         <v>68</v>
       </c>
@@ -3097,8 +3303,11 @@
       <c r="K69" s="7">
         <v>30.88</v>
       </c>
-    </row>
-    <row r="70" spans="1:11">
+      <c r="L69" s="10">
+        <v>33.200000000000003</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12">
       <c r="A70" t="s">
         <v>69</v>
       </c>
@@ -3123,8 +3332,11 @@
       <c r="K70" s="7">
         <v>30.94</v>
       </c>
-    </row>
-    <row r="71" spans="1:11">
+      <c r="L70" s="10">
+        <v>33.299999999999997</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12">
       <c r="A71" t="s">
         <v>70</v>
       </c>
@@ -3149,8 +3361,11 @@
       <c r="K71" s="7">
         <v>31.01</v>
       </c>
-    </row>
-    <row r="72" spans="1:11">
+      <c r="L71" s="10">
+        <v>33.4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12">
       <c r="A72" t="s">
         <v>71</v>
       </c>
@@ -3175,8 +3390,11 @@
       <c r="K72" s="7">
         <v>31.08</v>
       </c>
-    </row>
-    <row r="73" spans="1:11">
+      <c r="L72" s="10">
+        <v>33.5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12">
       <c r="A73" t="s">
         <v>72</v>
       </c>
@@ -3201,8 +3419,11 @@
       <c r="K73" s="7">
         <v>31.25</v>
       </c>
-    </row>
-    <row r="74" spans="1:11">
+      <c r="L73" s="10">
+        <v>33.5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12">
       <c r="A74" t="s">
         <v>73</v>
       </c>
@@ -3227,8 +3448,11 @@
       <c r="K74" s="7">
         <v>31.31</v>
       </c>
-    </row>
-    <row r="75" spans="1:11">
+      <c r="L74" s="10">
+        <v>33.700000000000003</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12">
       <c r="A75" t="s">
         <v>74</v>
       </c>
@@ -3253,8 +3477,11 @@
       <c r="K75" s="7">
         <v>31.61</v>
       </c>
-    </row>
-    <row r="76" spans="1:11">
+      <c r="L75" s="10">
+        <v>33.799999999999997</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12">
       <c r="A76" t="s">
         <v>75</v>
       </c>
@@ -3279,8 +3506,11 @@
       <c r="K76" s="7">
         <v>31.62</v>
       </c>
-    </row>
-    <row r="77" spans="1:11">
+      <c r="L76" s="10">
+        <v>33.9</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12">
       <c r="A77" t="s">
         <v>76</v>
       </c>
@@ -3305,8 +3535,11 @@
       <c r="K77" s="7">
         <v>31.85</v>
       </c>
-    </row>
-    <row r="78" spans="1:11">
+      <c r="L77" s="10">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12">
       <c r="A78" t="s">
         <v>77</v>
       </c>
@@ -3331,8 +3564,11 @@
       <c r="K78" s="7">
         <v>32.18</v>
       </c>
-    </row>
-    <row r="79" spans="1:11">
+      <c r="L78" s="10">
+        <v>34.200000000000003</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12">
       <c r="A79" t="s">
         <v>78</v>
       </c>
@@ -3357,8 +3593,11 @@
       <c r="K79" s="7">
         <v>32.380000000000003</v>
       </c>
-    </row>
-    <row r="80" spans="1:11">
+      <c r="L79" s="10">
+        <v>34.6</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12">
       <c r="A80" t="s">
         <v>79</v>
       </c>
@@ -3383,8 +3622,11 @@
       <c r="K80" s="7">
         <v>32.75</v>
       </c>
-    </row>
-    <row r="81" spans="1:11">
+      <c r="L80" s="10">
+        <v>34.9</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12">
       <c r="A81" t="s">
         <v>80</v>
       </c>
@@ -3409,8 +3651,11 @@
       <c r="K81" s="7">
         <v>32.92</v>
       </c>
-    </row>
-    <row r="82" spans="1:11">
+      <c r="L81" s="10">
+        <v>35.299999999999997</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12">
       <c r="A82" t="s">
         <v>81</v>
       </c>
@@ -3435,8 +3680,11 @@
       <c r="K82" s="7">
         <v>33</v>
       </c>
-    </row>
-    <row r="83" spans="1:11">
+      <c r="L82" s="10">
+        <v>35.5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12">
       <c r="A83" t="s">
         <v>82</v>
       </c>
@@ -3461,8 +3709,11 @@
       <c r="K83" s="7">
         <v>33.299999999999997</v>
       </c>
-    </row>
-    <row r="84" spans="1:11">
+      <c r="L83" s="10">
+        <v>35.700000000000003</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12">
       <c r="A84" t="s">
         <v>83</v>
       </c>
@@ -3487,8 +3738,11 @@
       <c r="K84" s="7">
         <v>33.6</v>
       </c>
-    </row>
-    <row r="85" spans="1:11">
+      <c r="L84" s="10">
+        <v>35.9</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12">
       <c r="A85" t="s">
         <v>84</v>
       </c>
@@ -3513,8 +3767,11 @@
       <c r="K85" s="7">
         <v>34</v>
       </c>
-    </row>
-    <row r="86" spans="1:11">
+      <c r="L85" s="10">
+        <v>36.4</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12">
       <c r="A86" t="s">
         <v>85</v>
       </c>
@@ -3539,8 +3796,11 @@
       <c r="K86" s="7">
         <v>34.299999999999997</v>
       </c>
-    </row>
-    <row r="87" spans="1:11">
+      <c r="L86" s="10">
+        <v>36.6</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12">
       <c r="A87" t="s">
         <v>86</v>
       </c>
@@ -3565,8 +3825,11 @@
       <c r="K87" s="7">
         <v>34.700000000000003</v>
       </c>
-    </row>
-    <row r="88" spans="1:11">
+      <c r="L87" s="10">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12">
       <c r="A88" t="s">
         <v>87</v>
       </c>
@@ -3591,8 +3854,11 @@
       <c r="K88" s="7">
         <v>35.1</v>
       </c>
-    </row>
-    <row r="89" spans="1:11">
+      <c r="L88" s="10">
+        <v>37.299999999999997</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12">
       <c r="A89" t="s">
         <v>88</v>
       </c>
@@ -3620,8 +3886,11 @@
       <c r="K89" s="7">
         <v>35.6</v>
       </c>
-    </row>
-    <row r="90" spans="1:11">
+      <c r="L89" s="10">
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12">
       <c r="A90" t="s">
         <v>89</v>
       </c>
@@ -3649,8 +3918,11 @@
       <c r="K90" s="7">
         <v>36.1</v>
       </c>
-    </row>
-    <row r="91" spans="1:11">
+      <c r="L90" s="10">
+        <v>37.799999999999997</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12">
       <c r="A91" t="s">
         <v>90</v>
       </c>
@@ -3678,8 +3950,11 @@
       <c r="K91" s="7">
         <v>36.6</v>
       </c>
-    </row>
-    <row r="92" spans="1:11">
+      <c r="L91" s="10">
+        <v>38.1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12">
       <c r="A92" t="s">
         <v>91</v>
       </c>
@@ -3707,8 +3982,11 @@
       <c r="K92" s="7">
         <v>37.1</v>
       </c>
-    </row>
-    <row r="93" spans="1:11">
+      <c r="L92" s="10">
+        <v>38.5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12">
       <c r="A93" t="s">
         <v>92</v>
       </c>
@@ -3736,8 +4014,11 @@
       <c r="K93" s="7">
         <v>37.700000000000003</v>
       </c>
-    </row>
-    <row r="94" spans="1:11">
+      <c r="L93" s="10">
+        <v>39.200000000000003</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12">
       <c r="A94" t="s">
         <v>93</v>
       </c>
@@ -3765,8 +4046,11 @@
       <c r="K94" s="7">
         <v>38.299999999999997</v>
       </c>
-    </row>
-    <row r="95" spans="1:11">
+      <c r="L94" s="10">
+        <v>39.6</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12">
       <c r="A95" t="s">
         <v>94</v>
       </c>
@@ -3794,8 +4078,11 @@
       <c r="K95" s="7">
         <v>38.799999999999997</v>
       </c>
-    </row>
-    <row r="96" spans="1:11">
+      <c r="L95" s="10">
+        <v>39.9</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12">
       <c r="A96" t="s">
         <v>95</v>
       </c>
@@ -3823,8 +4110,11 @@
       <c r="K96" s="7">
         <v>39.200000000000003</v>
       </c>
-    </row>
-    <row r="97" spans="1:11">
+      <c r="L96" s="10">
+        <v>40.299999999999997</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12">
       <c r="A97" t="s">
         <v>96</v>
       </c>
@@ -3852,8 +4142,11 @@
       <c r="K97" s="7">
         <v>39.799999999999997</v>
       </c>
-    </row>
-    <row r="98" spans="1:11">
+      <c r="L97" s="10">
+        <v>41.1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12">
       <c r="A98" t="s">
         <v>97</v>
       </c>
@@ -3881,8 +4174,11 @@
       <c r="K98" s="7">
         <v>40</v>
       </c>
-    </row>
-    <row r="99" spans="1:11">
+      <c r="L98" s="10">
+        <v>41.5</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12">
       <c r="A99" t="s">
         <v>98</v>
       </c>
@@ -3910,8 +4206,11 @@
       <c r="K99" s="7">
         <v>40.5</v>
       </c>
-    </row>
-    <row r="100" spans="1:11">
+      <c r="L99" s="10">
+        <v>41.7</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12">
       <c r="A100" t="s">
         <v>99</v>
       </c>
@@ -3939,8 +4238,11 @@
       <c r="K100" s="7">
         <v>40.799999999999997</v>
       </c>
-    </row>
-    <row r="101" spans="1:11">
+      <c r="L100" s="10">
+        <v>41.9</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12">
       <c r="A101" t="s">
         <v>100</v>
       </c>
@@ -3968,8 +4270,11 @@
       <c r="K101" s="7">
         <v>41.1</v>
       </c>
-    </row>
-    <row r="102" spans="1:11">
+      <c r="L101" s="10">
+        <v>42.1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12">
       <c r="A102" t="s">
         <v>101</v>
       </c>
@@ -3997,8 +4302,11 @@
       <c r="K102" s="7">
         <v>41.4</v>
       </c>
-    </row>
-    <row r="103" spans="1:11">
+      <c r="L102" s="10">
+        <v>42.6</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12">
       <c r="A103" t="s">
         <v>102</v>
       </c>
@@ -4026,8 +4334,11 @@
       <c r="K103" s="7">
         <v>41.7</v>
       </c>
-    </row>
-    <row r="104" spans="1:11">
+      <c r="L103" s="10">
+        <v>42.8</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12">
       <c r="A104" t="s">
         <v>103</v>
       </c>
@@ -4055,8 +4366,11 @@
       <c r="K104" s="7">
         <v>42.1</v>
       </c>
-    </row>
-    <row r="105" spans="1:11">
+      <c r="L104" s="10">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12">
       <c r="A105" t="s">
         <v>104</v>
       </c>
@@ -4084,8 +4398,11 @@
       <c r="K105" s="7">
         <v>42.5</v>
       </c>
-    </row>
-    <row r="106" spans="1:11">
+      <c r="L105" s="10">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12">
       <c r="A106" t="s">
         <v>105</v>
       </c>
@@ -4113,8 +4430,11 @@
       <c r="K106" s="7">
         <v>43.4</v>
       </c>
-    </row>
-    <row r="107" spans="1:11">
+      <c r="L106" s="10">
+        <v>43.6</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12">
       <c r="A107" t="s">
         <v>106</v>
       </c>
@@ -4142,8 +4462,11 @@
       <c r="K107" s="7">
         <v>44.2</v>
       </c>
-    </row>
-    <row r="108" spans="1:11">
+      <c r="L107" s="10">
+        <v>44.2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12">
       <c r="A108" t="s">
         <v>107</v>
       </c>
@@ -4171,8 +4494,11 @@
       <c r="K108" s="7">
         <v>45.2</v>
       </c>
-    </row>
-    <row r="109" spans="1:11">
+      <c r="L108" s="10">
+        <v>44.6</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12">
       <c r="A109" t="s">
         <v>108</v>
       </c>
@@ -4200,8 +4526,11 @@
       <c r="K109" s="7">
         <v>46.3</v>
       </c>
-    </row>
-    <row r="110" spans="1:11">
+      <c r="L109" s="10">
+        <v>45.3</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12">
       <c r="A110" t="s">
         <v>109</v>
       </c>
@@ -4229,8 +4558,11 @@
       <c r="K110" s="7">
         <v>47.8</v>
       </c>
-    </row>
-    <row r="111" spans="1:11">
+      <c r="L110" s="10">
+        <v>46.8</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12">
       <c r="A111" t="s">
         <v>110</v>
       </c>
@@ -4258,8 +4590,11 @@
       <c r="K111" s="7">
         <v>49</v>
       </c>
-    </row>
-    <row r="112" spans="1:11">
+      <c r="L111" s="10">
+        <v>49.7</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12">
       <c r="A112" t="s">
         <v>111</v>
       </c>
@@ -4287,8 +4622,11 @@
       <c r="K112" s="7">
         <v>50.6</v>
       </c>
-    </row>
-    <row r="113" spans="1:11">
+      <c r="L112" s="10">
+        <v>53.1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12">
       <c r="A113" t="s">
         <v>112</v>
       </c>
@@ -4316,8 +4654,11 @@
       <c r="K113" s="7">
         <v>51.9</v>
       </c>
-    </row>
-    <row r="114" spans="1:11">
+      <c r="L113" s="10">
+        <v>55.5</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12">
       <c r="A114" t="s">
         <v>113</v>
       </c>
@@ -4345,8 +4686,11 @@
       <c r="K114" s="7">
         <v>52.8</v>
       </c>
-    </row>
-    <row r="115" spans="1:11">
+      <c r="L114" s="10">
+        <v>57.2</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12">
       <c r="A115" t="s">
         <v>114</v>
       </c>
@@ -4374,8 +4718,11 @@
       <c r="K115" s="7">
         <v>53.5</v>
       </c>
-    </row>
-    <row r="116" spans="1:11">
+      <c r="L115" s="10">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12">
       <c r="A116" t="s">
         <v>115</v>
       </c>
@@ -4403,8 +4750,11 @@
       <c r="K116" s="7">
         <v>54.6</v>
       </c>
-    </row>
-    <row r="117" spans="1:11">
+      <c r="L116" s="10">
+        <v>58.9</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12">
       <c r="A117" t="s">
         <v>116</v>
       </c>
@@ -4432,8 +4782,11 @@
       <c r="K117" s="7">
         <v>55.6</v>
       </c>
-    </row>
-    <row r="118" spans="1:11">
+      <c r="L117" s="10">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12">
       <c r="A118" t="s">
         <v>117</v>
       </c>
@@ -4461,8 +4814,11 @@
       <c r="K118" s="7">
         <v>56</v>
       </c>
-    </row>
-    <row r="119" spans="1:11">
+      <c r="L118" s="10">
+        <v>61.1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12">
       <c r="A119" t="s">
         <v>118</v>
       </c>
@@ -4490,8 +4846,11 @@
       <c r="K119" s="7">
         <v>56.7</v>
       </c>
-    </row>
-    <row r="120" spans="1:11">
+      <c r="L119" s="10">
+        <v>61.8</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12">
       <c r="A120" t="s">
         <v>119</v>
       </c>
@@ -4519,8 +4878,11 @@
       <c r="K120" s="7">
         <v>57.6</v>
       </c>
-    </row>
-    <row r="121" spans="1:11">
+      <c r="L120" s="10">
+        <v>62.9</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12">
       <c r="A121" t="s">
         <v>120</v>
       </c>
@@ -4548,8 +4910,11 @@
       <c r="K121" s="7">
         <v>58.4</v>
       </c>
-    </row>
-    <row r="122" spans="1:11">
+      <c r="L121" s="10">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12">
       <c r="A122" t="s">
         <v>121</v>
       </c>
@@ -4577,8 +4942,11 @@
       <c r="K122" s="7">
         <v>59.6</v>
       </c>
-    </row>
-    <row r="123" spans="1:11">
+      <c r="L122" s="10">
+        <v>64.7</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12">
       <c r="A123" t="s">
         <v>122</v>
       </c>
@@ -4606,8 +4974,11 @@
       <c r="K123" s="7">
         <v>60.5</v>
       </c>
-    </row>
-    <row r="124" spans="1:11">
+      <c r="L123" s="10">
+        <v>65.7</v>
+      </c>
+    </row>
+    <row r="124" spans="1:12">
       <c r="A124" t="s">
         <v>123</v>
       </c>
@@ -4635,8 +5006,11 @@
       <c r="K124" s="7">
         <v>61.3</v>
       </c>
-    </row>
-    <row r="125" spans="1:11">
+      <c r="L124" s="10">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="125" spans="1:12">
       <c r="A125" t="s">
         <v>124</v>
       </c>
@@ -4664,8 +5038,11 @@
       <c r="K125" s="7">
         <v>62.3</v>
       </c>
-    </row>
-    <row r="126" spans="1:11">
+      <c r="L125" s="10">
+        <v>68.599999999999994</v>
+      </c>
+    </row>
+    <row r="126" spans="1:12">
       <c r="A126" t="s">
         <v>125</v>
       </c>
@@ -4696,8 +5073,11 @@
       <c r="K126" s="7">
         <v>63.4</v>
       </c>
-    </row>
-    <row r="127" spans="1:11">
+      <c r="L126" s="10">
+        <v>69.599999999999994</v>
+      </c>
+    </row>
+    <row r="127" spans="1:12">
       <c r="A127" t="s">
         <v>126</v>
       </c>
@@ -4728,8 +5108,11 @@
       <c r="K127" s="7">
         <v>65</v>
       </c>
-    </row>
-    <row r="128" spans="1:11">
+      <c r="L127" s="10">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="128" spans="1:12">
       <c r="A128" t="s">
         <v>127</v>
       </c>
@@ -4760,8 +5143,11 @@
       <c r="K128" s="7">
         <v>66.5</v>
       </c>
-    </row>
-    <row r="129" spans="1:11">
+      <c r="L128" s="10">
+        <v>72.599999999999994</v>
+      </c>
+    </row>
+    <row r="129" spans="1:12">
       <c r="A129" t="s">
         <v>128</v>
       </c>
@@ -4792,8 +5178,11 @@
       <c r="K129" s="7">
         <v>67.900000000000006</v>
       </c>
-    </row>
-    <row r="130" spans="1:11">
+      <c r="L129" s="10">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="130" spans="1:12">
       <c r="A130" t="s">
         <v>129</v>
       </c>
@@ -4824,8 +5213,11 @@
       <c r="K130" s="7">
         <v>69.900000000000006</v>
       </c>
-    </row>
-    <row r="131" spans="1:11">
+      <c r="L130" s="10">
+        <v>75.7</v>
+      </c>
+    </row>
+    <row r="131" spans="1:12">
       <c r="A131" t="s">
         <v>130</v>
       </c>
@@ -4856,8 +5248,11 @@
       <c r="K131" s="7">
         <v>72.2</v>
       </c>
-    </row>
-    <row r="132" spans="1:11">
+      <c r="L131" s="10">
+        <v>77.3</v>
+      </c>
+    </row>
+    <row r="132" spans="1:12">
       <c r="A132" t="s">
         <v>131</v>
       </c>
@@ -4888,8 +5283,11 @@
       <c r="K132" s="7">
         <v>74.400000000000006</v>
       </c>
-    </row>
-    <row r="133" spans="1:11">
+      <c r="L132" s="10">
+        <v>78.7</v>
+      </c>
+    </row>
+    <row r="133" spans="1:12">
       <c r="A133" t="s">
         <v>132</v>
       </c>
@@ -4920,8 +5318,11 @@
       <c r="K133" s="7">
         <v>76.900000000000006</v>
       </c>
-    </row>
-    <row r="134" spans="1:11">
+      <c r="L133" s="10">
+        <v>80.599999999999994</v>
+      </c>
+    </row>
+    <row r="134" spans="1:12">
       <c r="A134" t="s">
         <v>133</v>
       </c>
@@ -4952,8 +5353,11 @@
       <c r="K134" s="7">
         <v>80.099999999999994</v>
       </c>
-    </row>
-    <row r="135" spans="1:11">
+      <c r="L134" s="10">
+        <v>83.1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:12">
       <c r="A135" t="s">
         <v>134</v>
       </c>
@@ -4984,8 +5388,11 @@
       <c r="K135" s="7">
         <v>82.5</v>
       </c>
-    </row>
-    <row r="136" spans="1:11">
+      <c r="L135" s="10">
+        <v>85.1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:12">
       <c r="A136" t="s">
         <v>135</v>
       </c>
@@ -5016,8 +5423,11 @@
       <c r="K136" s="7">
         <v>83.9</v>
       </c>
-    </row>
-    <row r="137" spans="1:11">
+      <c r="L136" s="10">
+        <v>87.5</v>
+      </c>
+    </row>
+    <row r="137" spans="1:12">
       <c r="A137" t="s">
         <v>136</v>
       </c>
@@ -5048,8 +5458,11 @@
       <c r="K137" s="7">
         <v>86.4</v>
       </c>
-    </row>
-    <row r="138" spans="1:11">
+      <c r="L137" s="10">
+        <v>89.7</v>
+      </c>
+    </row>
+    <row r="138" spans="1:12">
       <c r="A138" t="s">
         <v>137</v>
       </c>
@@ -5080,8 +5493,11 @@
       <c r="K138" s="7">
         <v>88.6</v>
       </c>
-    </row>
-    <row r="139" spans="1:11">
+      <c r="L138" s="10">
+        <v>92.4</v>
+      </c>
+    </row>
+    <row r="139" spans="1:12">
       <c r="A139" t="s">
         <v>138</v>
       </c>
@@ -5112,8 +5528,11 @@
       <c r="K139" s="7">
         <v>90.5</v>
       </c>
-    </row>
-    <row r="140" spans="1:11">
+      <c r="L139" s="10">
+        <v>94.4</v>
+      </c>
+    </row>
+    <row r="140" spans="1:12">
       <c r="A140" t="s">
         <v>139</v>
       </c>
@@ -5144,8 +5563,11 @@
       <c r="K140" s="7">
         <v>93.1</v>
       </c>
-    </row>
-    <row r="141" spans="1:11">
+      <c r="L140" s="10">
+        <v>96.1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:12">
       <c r="A141" t="s">
         <v>140</v>
       </c>
@@ -5176,8 +5598,11 @@
       <c r="K141" s="7">
         <v>94.1</v>
       </c>
-    </row>
-    <row r="142" spans="1:11">
+      <c r="L141" s="10">
+        <v>98.1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:12">
       <c r="A142" t="s">
         <v>141</v>
       </c>
@@ -5208,8 +5633,11 @@
       <c r="K142" s="7">
         <v>94.7</v>
       </c>
-    </row>
-    <row r="143" spans="1:11">
+      <c r="L142" s="10">
+        <v>98.7</v>
+      </c>
+    </row>
+    <row r="143" spans="1:12">
       <c r="A143" t="s">
         <v>142</v>
       </c>
@@ -5240,8 +5668,11 @@
       <c r="K143" s="7">
         <v>97</v>
       </c>
-    </row>
-    <row r="144" spans="1:11">
+      <c r="L143" s="10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="144" spans="1:12">
       <c r="A144" t="s">
         <v>143</v>
       </c>
@@ -5272,8 +5703,11 @@
       <c r="K144" s="7">
         <v>97.7</v>
       </c>
-    </row>
-    <row r="145" spans="1:11">
+      <c r="L144" s="10">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="145" spans="1:12">
       <c r="A145" t="s">
         <v>144</v>
       </c>
@@ -5304,8 +5738,11 @@
       <c r="K145" s="7">
         <v>97.7</v>
       </c>
-    </row>
-    <row r="146" spans="1:11">
+      <c r="L145" s="10">
+        <v>101.9</v>
+      </c>
+    </row>
+    <row r="146" spans="1:12">
       <c r="A146" t="s">
         <v>145</v>
       </c>
@@ -5336,8 +5773,11 @@
       <c r="K146" s="7">
         <v>98.1</v>
       </c>
-    </row>
-    <row r="147" spans="1:11">
+      <c r="L146" s="10">
+        <v>102.2</v>
+      </c>
+    </row>
+    <row r="147" spans="1:12">
       <c r="A147" t="s">
         <v>146</v>
       </c>
@@ -5368,8 +5808,11 @@
       <c r="K147" s="7">
         <v>99.4</v>
       </c>
-    </row>
-    <row r="148" spans="1:11">
+      <c r="L147" s="10">
+        <v>102.6</v>
+      </c>
+    </row>
+    <row r="148" spans="1:12">
       <c r="A148" t="s">
         <v>147</v>
       </c>
@@ -5400,8 +5843,11 @@
       <c r="K148" s="7">
         <v>100.4</v>
       </c>
-    </row>
-    <row r="149" spans="1:11">
+      <c r="L148" s="10">
+        <v>103.3</v>
+      </c>
+    </row>
+    <row r="149" spans="1:12">
       <c r="A149" t="s">
         <v>148</v>
       </c>
@@ -5432,8 +5878,11 @@
       <c r="K149" s="7">
         <v>101.4</v>
       </c>
-    </row>
-    <row r="150" spans="1:11">
+      <c r="L149" s="10">
+        <v>103.8</v>
+      </c>
+    </row>
+    <row r="150" spans="1:12">
       <c r="A150" t="s">
         <v>149</v>
       </c>
@@ -5464,8 +5913,11 @@
       <c r="K150" s="7">
         <v>102.9</v>
       </c>
-    </row>
-    <row r="151" spans="1:11">
+      <c r="L150" s="10">
+        <v>104.6</v>
+      </c>
+    </row>
+    <row r="151" spans="1:12">
       <c r="A151" t="s">
         <v>150</v>
       </c>
@@ -5496,8 +5948,11 @@
       <c r="K151" s="7">
         <v>103.7</v>
       </c>
-    </row>
-    <row r="152" spans="1:11">
+      <c r="L151" s="10">
+        <v>105.2</v>
+      </c>
+    </row>
+    <row r="152" spans="1:12">
       <c r="A152" t="s">
         <v>151</v>
       </c>
@@ -5528,8 +5983,11 @@
       <c r="K152" s="7">
         <v>104.7</v>
       </c>
-    </row>
-    <row r="153" spans="1:11">
+      <c r="L152" s="10">
+        <v>105.9</v>
+      </c>
+    </row>
+    <row r="153" spans="1:12">
       <c r="A153" t="s">
         <v>152</v>
       </c>
@@ -5560,8 +6018,11 @@
       <c r="K153" s="7">
         <v>105.5</v>
       </c>
-    </row>
-    <row r="154" spans="1:11">
+      <c r="L153" s="10">
+        <v>105.6</v>
+      </c>
+    </row>
+    <row r="154" spans="1:12">
       <c r="A154" t="s">
         <v>153</v>
       </c>
@@ -5592,8 +6053,11 @@
       <c r="K154" s="7">
         <v>106.8</v>
       </c>
-    </row>
-    <row r="155" spans="1:11">
+      <c r="L154" s="10">
+        <v>107.1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:12">
       <c r="A155" t="s">
         <v>154</v>
       </c>
@@ -5624,8 +6088,11 @@
       <c r="K155" s="7">
         <v>107.5</v>
       </c>
-    </row>
-    <row r="156" spans="1:11">
+      <c r="L155" s="10">
+        <v>107.6</v>
+      </c>
+    </row>
+    <row r="156" spans="1:12">
       <c r="A156" t="s">
         <v>155</v>
       </c>
@@ -5656,8 +6123,11 @@
       <c r="K156" s="7">
         <v>108.1</v>
       </c>
-    </row>
-    <row r="157" spans="1:11">
+      <c r="L156" s="10">
+        <v>107.2</v>
+      </c>
+    </row>
+    <row r="157" spans="1:12">
       <c r="A157" t="s">
         <v>156</v>
       </c>
@@ -5688,8 +6158,11 @@
       <c r="K157" s="7">
         <v>109.5</v>
       </c>
-    </row>
-    <row r="158" spans="1:11">
+      <c r="L157" s="10">
+        <v>108.6</v>
+      </c>
+    </row>
+    <row r="158" spans="1:12">
       <c r="A158" t="s">
         <v>157</v>
       </c>
@@ -5720,8 +6193,11 @@
       <c r="K158" s="7">
         <v>109.1</v>
       </c>
-    </row>
-    <row r="159" spans="1:11">
+      <c r="L158" s="10">
+        <v>108.9</v>
+      </c>
+    </row>
+    <row r="159" spans="1:12">
       <c r="A159" t="s">
         <v>158</v>
       </c>
@@ -5752,8 +6228,11 @@
       <c r="K159" s="7">
         <v>109.4</v>
       </c>
-    </row>
-    <row r="160" spans="1:11">
+      <c r="L159" s="10">
+        <v>109.6</v>
+      </c>
+    </row>
+    <row r="160" spans="1:12">
       <c r="A160" t="s">
         <v>159</v>
       </c>
@@ -5784,8 +6263,11 @@
       <c r="K160" s="7">
         <v>110</v>
       </c>
-    </row>
-    <row r="161" spans="1:11">
+      <c r="L160" s="10">
+        <v>109.7</v>
+      </c>
+    </row>
+    <row r="161" spans="1:12">
       <c r="A161" t="s">
         <v>160</v>
       </c>
@@ -5816,8 +6298,11 @@
       <c r="K161" s="7">
         <v>110.8</v>
       </c>
-    </row>
-    <row r="162" spans="1:11">
+      <c r="L161" s="10">
+        <v>110.9</v>
+      </c>
+    </row>
+    <row r="162" spans="1:12">
       <c r="A162" t="s">
         <v>161</v>
       </c>
@@ -5848,8 +6333,11 @@
       <c r="K162" s="7">
         <v>112.2</v>
       </c>
-    </row>
-    <row r="163" spans="1:11">
+      <c r="L162" s="10">
+        <v>111.1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:12">
       <c r="A163" t="s">
         <v>162</v>
       </c>
@@ -5880,8 +6368,11 @@
       <c r="K163" s="7">
         <v>113.5</v>
       </c>
-    </row>
-    <row r="164" spans="1:11">
+      <c r="L163" s="10">
+        <v>111.5</v>
+      </c>
+    </row>
+    <row r="164" spans="1:12">
       <c r="A164" t="s">
         <v>163</v>
       </c>
@@ -5912,8 +6403,11 @@
       <c r="K164" s="7">
         <v>114.7</v>
       </c>
-    </row>
-    <row r="165" spans="1:11">
+      <c r="L164" s="10">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="165" spans="1:12">
       <c r="A165" t="s">
         <v>164</v>
       </c>
@@ -5944,8 +6438,11 @@
       <c r="K165" s="7">
         <v>115.6</v>
       </c>
-    </row>
-    <row r="166" spans="1:11">
+      <c r="L165" s="10">
+        <v>112.2</v>
+      </c>
+    </row>
+    <row r="166" spans="1:12">
       <c r="A166" t="s">
         <v>165</v>
       </c>
@@ -5976,8 +6473,11 @@
       <c r="K166" s="7">
         <v>116.5</v>
       </c>
-    </row>
-    <row r="167" spans="1:11">
+      <c r="L166" s="10">
+        <v>113.2</v>
+      </c>
+    </row>
+    <row r="167" spans="1:12">
       <c r="A167" t="s">
         <v>166</v>
       </c>
@@ -6008,8 +6508,11 @@
       <c r="K167" s="7">
         <v>118</v>
       </c>
-    </row>
-    <row r="168" spans="1:11">
+      <c r="L167" s="10">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="168" spans="1:12">
       <c r="A168" t="s">
         <v>167</v>
       </c>
@@ -6040,8 +6543,11 @@
       <c r="K168" s="7">
         <v>119.5</v>
       </c>
-    </row>
-    <row r="169" spans="1:11">
+      <c r="L168" s="10">
+        <v>115.2</v>
+      </c>
+    </row>
+    <row r="169" spans="1:12">
       <c r="A169" t="s">
         <v>168</v>
       </c>
@@ -6072,8 +6578,11 @@
       <c r="K169" s="7">
         <v>120.7</v>
       </c>
-    </row>
-    <row r="170" spans="1:11">
+      <c r="L169" s="10">
+        <v>116.1</v>
+      </c>
+    </row>
+    <row r="170" spans="1:12">
       <c r="A170" t="s">
         <v>169</v>
       </c>
@@ -6107,8 +6616,11 @@
       <c r="K170" s="7">
         <v>122.2</v>
       </c>
-    </row>
-    <row r="171" spans="1:11">
+      <c r="L170" s="10">
+        <v>117.5</v>
+      </c>
+    </row>
+    <row r="171" spans="1:12">
       <c r="A171" t="s">
         <v>170</v>
       </c>
@@ -6142,8 +6654,11 @@
       <c r="K171" s="7">
         <v>124.1</v>
       </c>
-    </row>
-    <row r="172" spans="1:11">
+      <c r="L171" s="10">
+        <v>118.9</v>
+      </c>
+    </row>
+    <row r="172" spans="1:12">
       <c r="A172" t="s">
         <v>171</v>
       </c>
@@ -6177,8 +6692,11 @@
       <c r="K172" s="7">
         <v>124.8</v>
       </c>
-    </row>
-    <row r="173" spans="1:11">
+      <c r="L172" s="10">
+        <v>119.7</v>
+      </c>
+    </row>
+    <row r="173" spans="1:12">
       <c r="A173" t="s">
         <v>172</v>
       </c>
@@ -6212,8 +6730,11 @@
       <c r="K173" s="7">
         <v>126.3</v>
       </c>
-    </row>
-    <row r="174" spans="1:11">
+      <c r="L173" s="10">
+        <v>120.6</v>
+      </c>
+    </row>
+    <row r="174" spans="1:12">
       <c r="A174" t="s">
         <v>173</v>
       </c>
@@ -6247,8 +6768,11 @@
       <c r="K174" s="7">
         <v>128.6</v>
       </c>
-    </row>
-    <row r="175" spans="1:11">
+      <c r="L174" s="10">
+        <v>121.8</v>
+      </c>
+    </row>
+    <row r="175" spans="1:12">
       <c r="A175" t="s">
         <v>174</v>
       </c>
@@ -6282,8 +6806,11 @@
       <c r="K175" s="7">
         <v>129.9</v>
       </c>
-    </row>
-    <row r="176" spans="1:11">
+      <c r="L175" s="10">
+        <v>122.5</v>
+      </c>
+    </row>
+    <row r="176" spans="1:12">
       <c r="A176" t="s">
         <v>175</v>
       </c>
@@ -6317,8 +6844,11 @@
       <c r="K176" s="7">
         <v>132.5</v>
       </c>
-    </row>
-    <row r="177" spans="1:11">
+      <c r="L176" s="10">
+        <v>123.8</v>
+      </c>
+    </row>
+    <row r="177" spans="1:12">
       <c r="A177" t="s">
         <v>176</v>
       </c>
@@ -6352,8 +6882,11 @@
       <c r="K177" s="7">
         <v>134.19999999999999</v>
       </c>
-    </row>
-    <row r="178" spans="1:11">
+      <c r="L177" s="10">
+        <v>124.8</v>
+      </c>
+    </row>
+    <row r="178" spans="1:12">
       <c r="A178" t="s">
         <v>177</v>
       </c>
@@ -6387,8 +6920,11 @@
       <c r="K178" s="7">
         <v>134.80000000000001</v>
       </c>
-    </row>
-    <row r="179" spans="1:11">
+      <c r="L178" s="10">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="179" spans="1:12">
       <c r="A179" t="s">
         <v>178</v>
       </c>
@@ -6422,8 +6958,11 @@
       <c r="K179" s="7">
         <v>136</v>
       </c>
-    </row>
-    <row r="180" spans="1:11">
+      <c r="L179" s="10">
+        <v>126.6</v>
+      </c>
+    </row>
+    <row r="180" spans="1:12">
       <c r="A180" t="s">
         <v>179</v>
       </c>
@@ -6457,8 +6996,11 @@
       <c r="K180" s="7">
         <v>137</v>
       </c>
-    </row>
-    <row r="181" spans="1:11">
+      <c r="L180" s="10">
+        <v>127.2</v>
+      </c>
+    </row>
+    <row r="181" spans="1:12">
       <c r="A181" t="s">
         <v>180</v>
       </c>
@@ -6492,8 +7034,11 @@
       <c r="K181" s="7">
         <v>138.19999999999999</v>
       </c>
-    </row>
-    <row r="182" spans="1:11">
+      <c r="L181" s="10">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="182" spans="1:12">
       <c r="A182" t="s">
         <v>181</v>
       </c>
@@ -6527,8 +7072,11 @@
       <c r="K182" s="7">
         <v>139.1</v>
       </c>
-    </row>
-    <row r="183" spans="1:11">
+      <c r="L182" s="10">
+        <v>128.6</v>
+      </c>
+    </row>
+    <row r="183" spans="1:12">
       <c r="A183" t="s">
         <v>182</v>
       </c>
@@ -6562,8 +7110,11 @@
       <c r="K183" s="7">
         <v>140.1</v>
       </c>
-    </row>
-    <row r="184" spans="1:11">
+      <c r="L183" s="10">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="184" spans="1:12">
       <c r="A184" t="s">
         <v>183</v>
       </c>
@@ -6597,8 +7148,11 @@
       <c r="K184" s="7">
         <v>141.1</v>
       </c>
-    </row>
-    <row r="185" spans="1:11">
+      <c r="L184" s="10">
+        <v>129.4</v>
+      </c>
+    </row>
+    <row r="185" spans="1:12">
       <c r="A185" t="s">
         <v>184</v>
       </c>
@@ -6632,8 +7186,11 @@
       <c r="K185" s="7">
         <v>142.30000000000001</v>
       </c>
-    </row>
-    <row r="186" spans="1:11">
+      <c r="L185" s="10">
+        <v>130.1</v>
+      </c>
+    </row>
+    <row r="186" spans="1:12">
       <c r="A186" t="s">
         <v>185</v>
       </c>
@@ -6667,8 +7224,11 @@
       <c r="K186" s="7">
         <v>143.30000000000001</v>
       </c>
-    </row>
-    <row r="187" spans="1:11">
+      <c r="L186" s="10">
+        <v>130.9</v>
+      </c>
+    </row>
+    <row r="187" spans="1:12">
       <c r="A187" t="s">
         <v>186</v>
       </c>
@@ -6702,8 +7262,11 @@
       <c r="K187" s="7">
         <v>144.30000000000001</v>
       </c>
-    </row>
-    <row r="188" spans="1:11">
+      <c r="L187" s="10">
+        <v>131.1</v>
+      </c>
+    </row>
+    <row r="188" spans="1:12">
       <c r="A188" t="s">
         <v>187</v>
       </c>
@@ -6737,8 +7300,11 @@
       <c r="K188" s="7">
         <v>145</v>
       </c>
-    </row>
-    <row r="189" spans="1:11">
+      <c r="L188" s="10">
+        <v>131.69999999999999</v>
+      </c>
+    </row>
+    <row r="189" spans="1:12">
       <c r="A189" t="s">
         <v>188</v>
       </c>
@@ -6772,8 +7338,11 @@
       <c r="K189" s="7">
         <v>146.30000000000001</v>
       </c>
-    </row>
-    <row r="190" spans="1:11">
+      <c r="L189" s="10">
+        <v>132.4</v>
+      </c>
+    </row>
+    <row r="190" spans="1:12">
       <c r="A190" t="s">
         <v>189</v>
       </c>
@@ -6807,8 +7376,11 @@
       <c r="K190" s="7">
         <v>147.1</v>
       </c>
-    </row>
-    <row r="191" spans="1:11">
+      <c r="L190" s="10">
+        <v>133.30000000000001</v>
+      </c>
+    </row>
+    <row r="191" spans="1:12">
       <c r="A191" t="s">
         <v>190</v>
       </c>
@@ -6842,8 +7414,11 @@
       <c r="K191" s="7">
         <v>147.9</v>
       </c>
-    </row>
-    <row r="192" spans="1:11">
+      <c r="L191" s="10">
+        <v>134.30000000000001</v>
+      </c>
+    </row>
+    <row r="192" spans="1:12">
       <c r="A192" t="s">
         <v>191</v>
       </c>
@@ -6877,8 +7452,11 @@
       <c r="K192" s="7">
         <v>149.30000000000001</v>
       </c>
-    </row>
-    <row r="193" spans="1:11">
+      <c r="L192" s="10">
+        <v>134.9</v>
+      </c>
+    </row>
+    <row r="193" spans="1:12">
       <c r="A193" t="s">
         <v>192</v>
       </c>
@@ -6912,8 +7490,11 @@
       <c r="K193" s="7">
         <v>150.1</v>
       </c>
-    </row>
-    <row r="194" spans="1:11">
+      <c r="L193" s="10">
+        <v>134.9</v>
+      </c>
+    </row>
+    <row r="194" spans="1:12">
       <c r="A194" t="s">
         <v>193</v>
       </c>
@@ -6947,8 +7528,11 @@
       <c r="K194" s="7">
         <v>151.19999999999999</v>
       </c>
-    </row>
-    <row r="195" spans="1:11">
+      <c r="L194" s="10">
+        <v>135.9</v>
+      </c>
+    </row>
+    <row r="195" spans="1:12">
       <c r="A195" t="s">
         <v>194</v>
       </c>
@@ -6982,8 +7566,11 @@
       <c r="K195" s="7">
         <v>152.4</v>
       </c>
-    </row>
-    <row r="196" spans="1:11">
+      <c r="L195" s="10">
+        <v>136.6</v>
+      </c>
+    </row>
+    <row r="196" spans="1:12">
       <c r="A196" t="s">
         <v>195</v>
       </c>
@@ -7017,8 +7604,11 @@
       <c r="K196" s="7">
         <v>153.1</v>
       </c>
-    </row>
-    <row r="197" spans="1:11">
+      <c r="L196" s="10">
+        <v>136.80000000000001</v>
+      </c>
+    </row>
+    <row r="197" spans="1:12">
       <c r="A197" t="s">
         <v>196</v>
       </c>
@@ -7052,8 +7642,11 @@
       <c r="K197" s="7">
         <v>153.9</v>
       </c>
-    </row>
-    <row r="198" spans="1:11">
+      <c r="L197" s="10">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="198" spans="1:12">
       <c r="A198" t="s">
         <v>197</v>
       </c>
@@ -7087,8 +7680,11 @@
       <c r="K198" s="7">
         <v>155.5</v>
       </c>
-    </row>
-    <row r="199" spans="1:11">
+      <c r="L198" s="10">
+        <v>138.1</v>
+      </c>
+    </row>
+    <row r="199" spans="1:12">
       <c r="A199" t="s">
         <v>198</v>
       </c>
@@ -7122,8 +7718,11 @@
       <c r="K199" s="7">
         <v>156.69999999999999</v>
       </c>
-    </row>
-    <row r="200" spans="1:11">
+      <c r="L199" s="10">
+        <v>138.4</v>
+      </c>
+    </row>
+    <row r="200" spans="1:12">
       <c r="A200" t="s">
         <v>199</v>
       </c>
@@ -7157,8 +7756,11 @@
       <c r="K200" s="7">
         <v>157.69999999999999</v>
       </c>
-    </row>
-    <row r="201" spans="1:11">
+      <c r="L200" s="10">
+        <v>138.4</v>
+      </c>
+    </row>
+    <row r="201" spans="1:12">
       <c r="A201" t="s">
         <v>200</v>
       </c>
@@ -7192,8 +7794,11 @@
       <c r="K201" s="7">
         <v>159.1</v>
       </c>
-    </row>
-    <row r="202" spans="1:11">
+      <c r="L201" s="10">
+        <v>138.4</v>
+      </c>
+    </row>
+    <row r="202" spans="1:12">
       <c r="A202" t="s">
         <v>201</v>
       </c>
@@ -7227,8 +7832,11 @@
       <c r="K202" s="7">
         <v>159.80000000000001</v>
       </c>
-    </row>
-    <row r="203" spans="1:11">
+      <c r="L202" s="10">
+        <v>138.6</v>
+      </c>
+    </row>
+    <row r="203" spans="1:12">
       <c r="A203" t="s">
         <v>202</v>
       </c>
@@ -7262,8 +7870,11 @@
       <c r="K203" s="7">
         <v>160.19999999999999</v>
       </c>
-    </row>
-    <row r="204" spans="1:11">
+      <c r="L203" s="10">
+        <v>138.30000000000001</v>
+      </c>
+    </row>
+    <row r="204" spans="1:12">
       <c r="A204" t="s">
         <v>203</v>
       </c>
@@ -7297,8 +7908,11 @@
       <c r="K204" s="7">
         <v>161.19999999999999</v>
       </c>
-    </row>
-    <row r="205" spans="1:11">
+      <c r="L204" s="10">
+        <v>138.19999999999999</v>
+      </c>
+    </row>
+    <row r="205" spans="1:12">
       <c r="A205" t="s">
         <v>204</v>
       </c>
@@ -7332,8 +7946,11 @@
       <c r="K205" s="7">
         <v>161.80000000000001</v>
       </c>
-    </row>
-    <row r="206" spans="1:11">
+      <c r="L205" s="10">
+        <v>137.69999999999999</v>
+      </c>
+    </row>
+    <row r="206" spans="1:12">
       <c r="A206" t="s">
         <v>205</v>
       </c>
@@ -7367,8 +7984,11 @@
       <c r="K206" s="7">
         <v>162</v>
       </c>
-    </row>
-    <row r="207" spans="1:11">
+      <c r="L206" s="10">
+        <v>137.80000000000001</v>
+      </c>
+    </row>
+    <row r="207" spans="1:12">
       <c r="A207" t="s">
         <v>206</v>
       </c>
@@ -7402,8 +8022,11 @@
       <c r="K207" s="7">
         <v>162.80000000000001</v>
       </c>
-    </row>
-    <row r="208" spans="1:11">
+      <c r="L207" s="10">
+        <v>137.4</v>
+      </c>
+    </row>
+    <row r="208" spans="1:12">
       <c r="A208" t="s">
         <v>207</v>
       </c>
@@ -7437,8 +8060,11 @@
       <c r="K208" s="7">
         <v>163.5</v>
       </c>
-    </row>
-    <row r="209" spans="1:11">
+      <c r="L208" s="10">
+        <v>137.5</v>
+      </c>
+    </row>
+    <row r="209" spans="1:12">
       <c r="A209" t="s">
         <v>208</v>
       </c>
@@ -7472,8 +8098,11 @@
       <c r="K209" s="7">
         <v>164.4</v>
       </c>
-    </row>
-    <row r="210" spans="1:11">
+      <c r="L209" s="10">
+        <v>137.5</v>
+      </c>
+    </row>
+    <row r="210" spans="1:12">
       <c r="A210" t="s">
         <v>209</v>
       </c>
@@ -7507,8 +8136,11 @@
       <c r="K210" s="7">
         <v>164.8</v>
       </c>
-    </row>
-    <row r="211" spans="1:11">
+      <c r="L210" s="10">
+        <v>137.6</v>
+      </c>
+    </row>
+    <row r="211" spans="1:12">
       <c r="A211" t="s">
         <v>210</v>
       </c>
@@ -7542,8 +8174,11 @@
       <c r="K211" s="7">
         <v>166</v>
       </c>
-    </row>
-    <row r="212" spans="1:11">
+      <c r="L211" s="10">
+        <v>137.5</v>
+      </c>
+    </row>
+    <row r="212" spans="1:12">
       <c r="A212" t="s">
         <v>211</v>
       </c>
@@ -7577,8 +8212,11 @@
       <c r="K212" s="7">
         <v>167.8</v>
       </c>
-    </row>
-    <row r="213" spans="1:11">
+      <c r="L212" s="10">
+        <v>137.4</v>
+      </c>
+    </row>
+    <row r="213" spans="1:12">
       <c r="A213" t="s">
         <v>212</v>
       </c>
@@ -7612,8 +8250,11 @@
       <c r="K213" s="7">
         <v>168.8</v>
       </c>
-    </row>
-    <row r="214" spans="1:11">
+      <c r="L213" s="10">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="214" spans="1:12">
       <c r="A214" t="s">
         <v>213</v>
       </c>
@@ -7647,8 +8288,11 @@
       <c r="K214" s="7">
         <v>171</v>
       </c>
-    </row>
-    <row r="215" spans="1:11">
+      <c r="L214" s="10">
+        <v>138.4</v>
+      </c>
+    </row>
+    <row r="215" spans="1:12">
       <c r="A215" t="s">
         <v>214</v>
       </c>
@@ -7682,8 +8326,11 @@
       <c r="K215" s="7">
         <v>172.2</v>
       </c>
-    </row>
-    <row r="216" spans="1:11">
+      <c r="L215" s="10">
+        <v>138.80000000000001</v>
+      </c>
+    </row>
+    <row r="216" spans="1:12">
       <c r="A216" t="s">
         <v>215</v>
       </c>
@@ -7717,8 +8364,11 @@
       <c r="K216" s="7">
         <v>173.6</v>
       </c>
-    </row>
-    <row r="217" spans="1:11">
+      <c r="L216" s="10">
+        <v>139.30000000000001</v>
+      </c>
+    </row>
+    <row r="217" spans="1:12">
       <c r="A217" t="s">
         <v>216</v>
       </c>
@@ -7752,8 +8402,11 @@
       <c r="K217" s="7">
         <v>174.6</v>
       </c>
-    </row>
-    <row r="218" spans="1:11">
+      <c r="L217" s="10">
+        <v>139.5</v>
+      </c>
+    </row>
+    <row r="218" spans="1:12">
       <c r="A218" t="s">
         <v>217</v>
       </c>
@@ -7787,8 +8440,11 @@
       <c r="K218" s="7">
         <v>176.1</v>
       </c>
-    </row>
-    <row r="219" spans="1:11">
+      <c r="L218" s="10">
+        <v>139.6</v>
+      </c>
+    </row>
+    <row r="219" spans="1:12">
       <c r="A219" t="s">
         <v>218</v>
       </c>
@@ -7822,8 +8478,11 @@
       <c r="K219" s="7">
         <v>177.7</v>
       </c>
-    </row>
-    <row r="220" spans="1:11">
+      <c r="L219" s="10">
+        <v>139.80000000000001</v>
+      </c>
+    </row>
+    <row r="220" spans="1:12">
       <c r="A220" t="s">
         <v>219</v>
       </c>
@@ -7857,8 +8516,11 @@
       <c r="K220" s="7">
         <v>178.1</v>
       </c>
-    </row>
-    <row r="221" spans="1:11">
+      <c r="L220" s="10">
+        <v>140.19999999999999</v>
+      </c>
+    </row>
+    <row r="221" spans="1:12">
       <c r="A221" t="s">
         <v>220</v>
       </c>
@@ -7892,8 +8554,11 @@
       <c r="K221" s="7">
         <v>177.4</v>
       </c>
-    </row>
-    <row r="222" spans="1:11">
+      <c r="L221" s="10">
+        <v>139.6</v>
+      </c>
+    </row>
+    <row r="222" spans="1:12">
       <c r="A222" t="s">
         <v>221</v>
       </c>
@@ -7927,8 +8592,11 @@
       <c r="K222" s="7">
         <v>178.5</v>
       </c>
-    </row>
-    <row r="223" spans="1:11">
+      <c r="L222" s="10">
+        <v>139.4</v>
+      </c>
+    </row>
+    <row r="223" spans="1:12">
       <c r="A223" t="s">
         <v>222</v>
       </c>
@@ -7962,8 +8630,11 @@
       <c r="K223" s="7">
         <v>179.6</v>
       </c>
-    </row>
-    <row r="224" spans="1:11">
+      <c r="L223" s="10">
+        <v>139.30000000000001</v>
+      </c>
+    </row>
+    <row r="224" spans="1:12">
       <c r="A224" t="s">
         <v>223</v>
       </c>
@@ -7997,8 +8668,11 @@
       <c r="K224" s="7">
         <v>180.8</v>
       </c>
-    </row>
-    <row r="225" spans="1:11">
+      <c r="L224" s="10">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="225" spans="1:12">
       <c r="A225" t="s">
         <v>224</v>
       </c>
@@ -8032,8 +8706,11 @@
       <c r="K225" s="7">
         <v>181.8</v>
       </c>
-    </row>
-    <row r="226" spans="1:11">
+      <c r="L225" s="10">
+        <v>138.80000000000001</v>
+      </c>
+    </row>
+    <row r="226" spans="1:12">
       <c r="A226" t="s">
         <v>225</v>
       </c>
@@ -8067,8 +8744,11 @@
       <c r="K226" s="7">
         <v>183.9</v>
       </c>
-    </row>
-    <row r="227" spans="1:11">
+      <c r="L226" s="10">
+        <v>139.80000000000001</v>
+      </c>
+    </row>
+    <row r="227" spans="1:12">
       <c r="A227" t="s">
         <v>226</v>
       </c>
@@ -8102,8 +8782,11 @@
       <c r="K227" s="7">
         <v>183.1</v>
       </c>
-    </row>
-    <row r="228" spans="1:11">
+      <c r="L227" s="10">
+        <v>139.30000000000001</v>
+      </c>
+    </row>
+    <row r="228" spans="1:12">
       <c r="A228" t="s">
         <v>227</v>
       </c>
@@ -8137,8 +8820,11 @@
       <c r="K228" s="7">
         <v>185.1</v>
       </c>
-    </row>
-    <row r="229" spans="1:11">
+      <c r="L228" s="10">
+        <v>139.6</v>
+      </c>
+    </row>
+    <row r="229" spans="1:12">
       <c r="A229" t="s">
         <v>228</v>
       </c>
@@ -8172,8 +8858,11 @@
       <c r="K229" s="7">
         <v>185.5</v>
       </c>
-    </row>
-    <row r="230" spans="1:11">
+      <c r="L229" s="10">
+        <v>139.9</v>
+      </c>
+    </row>
+    <row r="230" spans="1:12">
       <c r="A230" t="s">
         <v>229</v>
       </c>
@@ -8207,8 +8896,11 @@
       <c r="K230" s="7">
         <v>187.1</v>
       </c>
-    </row>
-    <row r="231" spans="1:11">
+      <c r="L230" s="10">
+        <v>140.4</v>
+      </c>
+    </row>
+    <row r="231" spans="1:12">
       <c r="A231" t="s">
         <v>230</v>
       </c>
@@ -8242,8 +8934,11 @@
       <c r="K231" s="7">
         <v>188.9</v>
       </c>
-    </row>
-    <row r="232" spans="1:11">
+      <c r="L231" s="10">
+        <v>141.6</v>
+      </c>
+    </row>
+    <row r="232" spans="1:12">
       <c r="A232" t="s">
         <v>231</v>
       </c>
@@ -8277,8 +8972,11 @@
       <c r="K232" s="7">
         <v>189.8</v>
       </c>
-    </row>
-    <row r="233" spans="1:11">
+      <c r="L232" s="10">
+        <v>142.1</v>
+      </c>
+    </row>
+    <row r="233" spans="1:12">
       <c r="A233" t="s">
         <v>232</v>
       </c>
@@ -8312,8 +9010,11 @@
       <c r="K233" s="7">
         <v>191.7</v>
       </c>
-    </row>
-    <row r="234" spans="1:11">
+      <c r="L233" s="10">
+        <v>143.30000000000001</v>
+      </c>
+    </row>
+    <row r="234" spans="1:12">
       <c r="A234" t="s">
         <v>233</v>
       </c>
@@ -8347,8 +9048,11 @@
       <c r="K234" s="7">
         <v>193.1</v>
       </c>
-    </row>
-    <row r="235" spans="1:11">
+      <c r="L234" s="10">
+        <v>144.1</v>
+      </c>
+    </row>
+    <row r="235" spans="1:12">
       <c r="A235" t="s">
         <v>234</v>
       </c>
@@ -8382,8 +9086,11 @@
       <c r="K235" s="7">
         <v>193.7</v>
       </c>
-    </row>
-    <row r="236" spans="1:11">
+      <c r="L235" s="10">
+        <v>144.6</v>
+      </c>
+    </row>
+    <row r="236" spans="1:12">
       <c r="A236" t="s">
         <v>235</v>
       </c>
@@ -8417,8 +9124,11 @@
       <c r="K236" s="7">
         <v>198.8</v>
       </c>
-    </row>
-    <row r="237" spans="1:11">
+      <c r="L236" s="10">
+        <v>145.30000000000001</v>
+      </c>
+    </row>
+    <row r="237" spans="1:12">
       <c r="A237" t="s">
         <v>236</v>
       </c>
@@ -8452,8 +9162,11 @@
       <c r="K237" s="7">
         <v>198.1</v>
       </c>
-    </row>
-    <row r="238" spans="1:11">
+      <c r="L237" s="10">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="238" spans="1:12">
       <c r="A238" t="s">
         <v>237</v>
       </c>
@@ -8487,8 +9200,11 @@
       <c r="K238" s="7">
         <v>199.7</v>
       </c>
-    </row>
-    <row r="239" spans="1:11">
+      <c r="L238" s="10">
+        <v>146.30000000000001</v>
+      </c>
+    </row>
+    <row r="239" spans="1:12">
       <c r="A239" t="s">
         <v>238</v>
       </c>
@@ -8522,8 +9238,11 @@
       <c r="K239" s="7">
         <v>201.8</v>
       </c>
-    </row>
-    <row r="240" spans="1:11">
+      <c r="L239" s="10">
+        <v>147.1</v>
+      </c>
+    </row>
+    <row r="240" spans="1:12">
       <c r="A240" t="s">
         <v>239</v>
       </c>
@@ -8557,8 +9276,11 @@
       <c r="K240" s="7">
         <v>202.8</v>
       </c>
-    </row>
-    <row r="241" spans="1:11">
+      <c r="L240" s="10">
+        <v>147.5</v>
+      </c>
+    </row>
+    <row r="241" spans="1:12">
       <c r="A241" t="s">
         <v>240</v>
       </c>
@@ -8592,8 +9314,11 @@
       <c r="K241" s="7">
         <v>203.1</v>
       </c>
-    </row>
-    <row r="242" spans="1:11">
+      <c r="L241" s="10">
+        <v>148.30000000000001</v>
+      </c>
+    </row>
+    <row r="242" spans="1:12">
       <c r="A242" t="s">
         <v>241</v>
       </c>
@@ -8627,8 +9352,11 @@
       <c r="K242" s="7">
         <v>205.28800000000001</v>
       </c>
-    </row>
-    <row r="243" spans="1:11">
+      <c r="L242" s="10">
+        <v>149.1</v>
+      </c>
+    </row>
+    <row r="243" spans="1:12">
       <c r="A243" t="s">
         <v>242</v>
       </c>
@@ -8662,8 +9390,11 @@
       <c r="K243" s="7">
         <v>207.23400000000001</v>
       </c>
-    </row>
-    <row r="244" spans="1:11">
+      <c r="L243" s="10">
+        <v>149.5</v>
+      </c>
+    </row>
+    <row r="244" spans="1:12">
       <c r="A244" t="s">
         <v>243</v>
       </c>
@@ -8697,8 +9428,11 @@
       <c r="K244" s="7">
         <v>208.547</v>
       </c>
-    </row>
-    <row r="245" spans="1:11">
+      <c r="L244" s="10">
+        <v>149.80000000000001</v>
+      </c>
+    </row>
+    <row r="245" spans="1:12">
       <c r="A245" t="s">
         <v>244</v>
       </c>
@@ -8732,8 +9466,11 @@
       <c r="K245" s="7">
         <v>211.44499999999999</v>
       </c>
-    </row>
-    <row r="246" spans="1:11">
+      <c r="L245" s="10">
+        <v>150.5</v>
+      </c>
+    </row>
+    <row r="246" spans="1:12">
       <c r="A246" t="s">
         <v>245</v>
       </c>
@@ -8767,8 +9504,11 @@
       <c r="K246" s="7">
         <v>213.44800000000001</v>
       </c>
-    </row>
-    <row r="247" spans="1:11">
+      <c r="L246" s="10">
+        <v>151.9</v>
+      </c>
+    </row>
+    <row r="247" spans="1:12">
       <c r="A247" t="s">
         <v>246</v>
       </c>
@@ -8802,8 +9542,11 @@
       <c r="K247" s="7">
         <v>217.46299999999999</v>
       </c>
-    </row>
-    <row r="248" spans="1:11">
+      <c r="L247" s="10">
+        <v>153.19999999999999</v>
+      </c>
+    </row>
+    <row r="248" spans="1:12">
       <c r="A248" t="s">
         <v>247</v>
       </c>
@@ -8837,8 +9580,11 @@
       <c r="K248" s="7">
         <v>218.87700000000001</v>
       </c>
-    </row>
-    <row r="249" spans="1:11">
+      <c r="L248" s="10">
+        <v>155.1</v>
+      </c>
+    </row>
+    <row r="249" spans="1:12">
       <c r="A249" t="s">
         <v>248</v>
       </c>
@@ -8872,8 +9618,11 @@
       <c r="K249" s="7">
         <v>211.398</v>
       </c>
-    </row>
-    <row r="250" spans="1:11">
+      <c r="L249" s="10">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="250" spans="1:12">
       <c r="A250" t="s">
         <v>249</v>
       </c>
@@ -8907,8 +9656,11 @@
       <c r="K250" s="7">
         <v>212.495</v>
       </c>
-    </row>
-    <row r="251" spans="1:11">
+      <c r="L250" s="10">
+        <v>156.80000000000001</v>
+      </c>
+    </row>
+    <row r="251" spans="1:12">
       <c r="A251" t="s">
         <v>250</v>
       </c>
@@ -8942,8 +9694,11 @@
       <c r="K251" s="7">
         <v>214.79</v>
       </c>
-    </row>
-    <row r="252" spans="1:11">
+      <c r="L251" s="10">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="252" spans="1:12">
       <c r="A252" t="s">
         <v>251</v>
       </c>
@@ -8977,8 +9732,11 @@
       <c r="K252" s="7">
         <v>215.86099999999999</v>
       </c>
-    </row>
-    <row r="253" spans="1:11">
+      <c r="L252" s="10">
+        <v>156.69999999999999</v>
+      </c>
+    </row>
+    <row r="253" spans="1:12">
       <c r="A253" t="s">
         <v>252</v>
       </c>
@@ -9012,8 +9770,11 @@
       <c r="K253" s="7">
         <v>217.34700000000001</v>
       </c>
-    </row>
-    <row r="254" spans="1:11">
+      <c r="L253" s="10">
+        <v>156.80000000000001</v>
+      </c>
+    </row>
+    <row r="254" spans="1:12">
       <c r="A254" t="s">
         <v>253</v>
       </c>
@@ -9047,8 +9808,11 @@
       <c r="K254" s="7">
         <v>217.35300000000001</v>
       </c>
-    </row>
-    <row r="255" spans="1:11">
+      <c r="L254" s="10">
+        <v>157.1</v>
+      </c>
+    </row>
+    <row r="255" spans="1:12">
       <c r="A255" t="s">
         <v>254</v>
       </c>
@@ -9082,8 +9846,11 @@
       <c r="K255" s="7">
         <v>217.19900000000001</v>
       </c>
-    </row>
-    <row r="256" spans="1:11">
+      <c r="L255" s="10">
+        <v>157.30000000000001</v>
+      </c>
+    </row>
+    <row r="256" spans="1:12">
       <c r="A256" t="s">
         <v>255</v>
       </c>
@@ -9117,8 +9884,11 @@
       <c r="K256" s="7">
         <v>218.27500000000001</v>
       </c>
-    </row>
-    <row r="257" spans="1:11">
+      <c r="L256" s="10">
+        <v>157.69999999999999</v>
+      </c>
+    </row>
+    <row r="257" spans="1:12">
       <c r="A257" t="s">
         <v>256</v>
       </c>
@@ -9152,8 +9922,11 @@
       <c r="K257" s="7">
         <v>220.47200000000001</v>
       </c>
-    </row>
-    <row r="258" spans="1:11">
+      <c r="L257" s="10">
+        <v>157.5</v>
+      </c>
+    </row>
+    <row r="258" spans="1:12">
       <c r="A258" t="s">
         <v>257</v>
       </c>
@@ -9187,8 +9960,11 @@
       <c r="K258" s="7">
         <v>223.04599999999999</v>
       </c>
-    </row>
-    <row r="259" spans="1:11">
+      <c r="L258" s="10">
+        <v>158.69999999999999</v>
+      </c>
+    </row>
+    <row r="259" spans="1:12">
       <c r="A259" t="s">
         <v>258</v>
       </c>
@@ -9222,8 +9998,11 @@
       <c r="K259" s="7">
         <v>224.80600000000001</v>
       </c>
-    </row>
-    <row r="260" spans="1:11">
+      <c r="L259" s="10">
+        <v>159.80000000000001</v>
+      </c>
+    </row>
+    <row r="260" spans="1:12">
       <c r="A260" t="s">
         <v>259</v>
       </c>
@@ -9257,8 +10036,11 @@
       <c r="K260" s="7">
         <v>226.59700000000001</v>
       </c>
-    </row>
-    <row r="261" spans="1:11">
+      <c r="L260" s="10">
+        <v>160.4</v>
+      </c>
+    </row>
+    <row r="261" spans="1:12">
       <c r="A261" t="s">
         <v>260</v>
       </c>
@@ -9292,8 +10074,11 @@
       <c r="K261" s="7">
         <v>227.22300000000001</v>
       </c>
-    </row>
-    <row r="262" spans="1:11">
+      <c r="L261" s="10">
+        <v>161.19999999999999</v>
+      </c>
+    </row>
+    <row r="262" spans="1:12">
       <c r="A262" t="s">
         <v>261</v>
       </c>
@@ -9327,8 +10112,11 @@
       <c r="K262" s="7">
         <v>228.80699999999999</v>
       </c>
-    </row>
-    <row r="263" spans="1:11">
+      <c r="L262" s="10">
+        <v>162.19999999999999</v>
+      </c>
+    </row>
+    <row r="263" spans="1:12">
       <c r="A263" t="s">
         <v>262</v>
       </c>
@@ -9362,8 +10150,11 @@
       <c r="K263" s="7">
         <v>228.524</v>
       </c>
-    </row>
-    <row r="264" spans="1:11">
+      <c r="L263" s="10">
+        <v>162.80000000000001</v>
+      </c>
+    </row>
+    <row r="264" spans="1:12">
       <c r="A264" t="s">
         <v>263</v>
       </c>
@@ -9397,8 +10188,11 @@
       <c r="K264" s="7">
         <v>231.01499999999999</v>
       </c>
-    </row>
-    <row r="265" spans="1:11">
+      <c r="L264" s="10">
+        <v>163.19999999999999</v>
+      </c>
+    </row>
+    <row r="265" spans="1:12">
       <c r="A265" t="s">
         <v>264</v>
       </c>
@@ -9432,8 +10226,11 @@
       <c r="K265" s="7">
         <v>231.221</v>
       </c>
-    </row>
-    <row r="266" spans="1:11">
+      <c r="L265" s="10">
+        <v>163.30000000000001</v>
+      </c>
+    </row>
+    <row r="266" spans="1:12">
       <c r="A266" t="s">
         <v>265</v>
       </c>
@@ -9467,8 +10264,11 @@
       <c r="K266" s="7">
         <v>232.29900000000001</v>
       </c>
-    </row>
-    <row r="267" spans="1:11">
+      <c r="L266" s="10">
+        <v>163.69999999999999</v>
+      </c>
+    </row>
+    <row r="267" spans="1:12">
       <c r="A267" t="s">
         <v>266</v>
       </c>
@@ -9502,8 +10302,11 @@
       <c r="K267" s="7">
         <v>232.374</v>
       </c>
-    </row>
-    <row r="268" spans="1:11">
+      <c r="L267" s="10">
+        <v>164.1</v>
+      </c>
+    </row>
+    <row r="268" spans="1:12">
       <c r="A268" t="s">
         <v>267</v>
       </c>
@@ -9537,8 +10340,11 @@
       <c r="K268" s="7">
         <v>233.63200000000001</v>
       </c>
-    </row>
-    <row r="269" spans="1:11">
+      <c r="L268" s="10">
+        <v>164.6</v>
+      </c>
+    </row>
+    <row r="269" spans="1:12">
       <c r="A269" t="s">
         <v>268</v>
       </c>
@@ -9572,8 +10378,11 @@
       <c r="K269" s="7">
         <v>234.72300000000001</v>
       </c>
-    </row>
-    <row r="270" spans="1:11">
+      <c r="L269" s="10">
+        <v>165.4</v>
+      </c>
+    </row>
+    <row r="270" spans="1:12">
       <c r="A270" t="s">
         <v>269</v>
       </c>
@@ -9607,8 +10416,11 @@
       <c r="K270" s="7">
         <v>235.97800000000001</v>
       </c>
-    </row>
-    <row r="271" spans="1:11">
+      <c r="L270" s="10">
+        <v>165.9</v>
+      </c>
+    </row>
+    <row r="271" spans="1:12">
       <c r="A271" t="s">
         <v>270</v>
       </c>
@@ -9642,8 +10454,11 @@
       <c r="K271" s="7">
         <v>237.029</v>
       </c>
-    </row>
-    <row r="272" spans="1:11">
+      <c r="L271" s="10">
+        <v>166.4</v>
+      </c>
+    </row>
+    <row r="272" spans="1:12">
       <c r="A272" t="s">
         <v>271</v>
       </c>
@@ -9677,8 +10492,11 @@
       <c r="K272" s="7">
         <v>237.48599999999999</v>
       </c>
-    </row>
-    <row r="273" spans="1:11">
+      <c r="L272" s="10">
+        <v>166.8</v>
+      </c>
+    </row>
+    <row r="273" spans="1:12">
       <c r="A273" t="s">
         <v>272</v>
       </c>
@@ -9712,8 +10530,11 @@
       <c r="K273" s="7">
         <v>236.29</v>
       </c>
-    </row>
-    <row r="274" spans="1:11">
+      <c r="L273" s="10">
+        <v>166.9</v>
+      </c>
+    </row>
+    <row r="274" spans="1:12">
       <c r="A274" t="s">
         <v>273</v>
       </c>
@@ -9747,8 +10568,11 @@
       <c r="K274" s="7">
         <v>235.989</v>
       </c>
-    </row>
-    <row r="275" spans="1:11">
+      <c r="L274" s="10">
+        <v>168.3</v>
+      </c>
+    </row>
+    <row r="275" spans="1:12">
       <c r="A275" t="s">
         <v>274</v>
       </c>
@@ -9782,8 +10606,11 @@
       <c r="K275" s="7">
         <v>237.41900000000001</v>
       </c>
-    </row>
-    <row r="276" spans="1:11">
+      <c r="L275" s="10">
+        <v>168.5</v>
+      </c>
+    </row>
+    <row r="276" spans="1:12">
       <c r="A276" t="s">
         <v>275</v>
       </c>
@@ -9817,8 +10644,11 @@
       <c r="K276" s="7">
         <v>237.46700000000001</v>
       </c>
-    </row>
-    <row r="277" spans="1:11">
+      <c r="L276" s="10">
+        <v>168.9</v>
+      </c>
+    </row>
+    <row r="277" spans="1:12">
       <c r="A277" t="s">
         <v>276</v>
       </c>
@@ -9852,8 +10682,11 @@
       <c r="K277" s="7">
         <v>237.846</v>
       </c>
-    </row>
-    <row r="278" spans="1:11">
+      <c r="L277" s="10">
+        <v>168.8</v>
+      </c>
+    </row>
+    <row r="278" spans="1:12">
       <c r="A278" t="s">
         <v>277</v>
       </c>
@@ -9887,8 +10720,11 @@
       <c r="K278" s="7">
         <v>238.078</v>
       </c>
-    </row>
-    <row r="279" spans="1:11">
+      <c r="L278" s="10">
+        <v>168.9</v>
+      </c>
+    </row>
+    <row r="279" spans="1:12">
       <c r="A279" t="s">
         <v>278</v>
       </c>
@@ -9922,8 +10758,11 @@
       <c r="K279" s="7">
         <v>239.84200000000001</v>
       </c>
-    </row>
-    <row r="280" spans="1:11">
+      <c r="L279" s="10">
+        <v>169.5</v>
+      </c>
+    </row>
+    <row r="280" spans="1:12">
       <c r="A280" t="s">
         <v>279</v>
       </c>
@@ -9957,8 +10796,11 @@
       <c r="K280" s="7">
         <v>241.006</v>
       </c>
-    </row>
-    <row r="281" spans="1:11">
+      <c r="L280" s="10">
+        <v>169.5</v>
+      </c>
+    </row>
+    <row r="281" spans="1:12">
       <c r="A281" t="s">
         <v>280</v>
       </c>
@@ -9992,8 +10834,11 @@
       <c r="K281" s="7">
         <v>242.821</v>
       </c>
-    </row>
-    <row r="282" spans="1:11">
+      <c r="L281" s="10">
+        <v>169.9</v>
+      </c>
+    </row>
+    <row r="282" spans="1:12">
       <c r="A282" t="s">
         <v>281</v>
       </c>
@@ -10027,8 +10872,11 @@
       <c r="K282" s="7">
         <v>243.75200000000001</v>
       </c>
-    </row>
-    <row r="283" spans="1:11">
+      <c r="L282" s="10">
+        <v>170.6</v>
+      </c>
+    </row>
+    <row r="283" spans="1:12">
       <c r="A283" t="s">
         <v>282</v>
       </c>
@@ -10062,21 +10910,27 @@
       <c r="K283" s="7">
         <v>243.79</v>
       </c>
-    </row>
-    <row r="284" spans="1:11">
+      <c r="L283" s="10">
+        <v>170.9</v>
+      </c>
+    </row>
+    <row r="284" spans="1:12">
       <c r="B284" s="2"/>
       <c r="D284" s="4"/>
-    </row>
-    <row r="285" spans="1:11">
+      <c r="L284" s="10">
+        <v>171.2</v>
+      </c>
+    </row>
+    <row r="285" spans="1:12">
       <c r="B285" s="2"/>
     </row>
-    <row r="286" spans="1:11">
+    <row r="286" spans="1:12">
       <c r="B286" s="2"/>
     </row>
-    <row r="287" spans="1:11">
+    <row r="287" spans="1:12">
       <c r="B287" s="2"/>
     </row>
-    <row r="288" spans="1:11">
+    <row r="288" spans="1:12">
       <c r="B288" s="2"/>
     </row>
     <row r="289" spans="2:2">

</xml_diff>